<commit_message>
dev of alliance region
</commit_message>
<xml_diff>
--- a/gameData/shared/AllianceBuilding.xlsx
+++ b/gameData/shared/AllianceBuilding.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6460" yWindow="5660" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="4480" yWindow="1940" windowWidth="25600" windowHeight="17000" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="palace" sheetId="1" r:id="rId1"/>
     <sheet name="moonGate" sheetId="2" r:id="rId2"/>
     <sheet name="orderHall" sheetId="3" r:id="rId3"/>
     <sheet name="shrine" sheetId="4" r:id="rId4"/>
-    <sheet name="allianceShop" sheetId="5" r:id="rId5"/>
+    <sheet name="shop" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -1678,8 +1678,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -1968,8 +1968,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>

</xml_diff>